<commit_message>
updating conversion efficiency file
</commit_message>
<xml_diff>
--- a/metadata/lambda_conversion.xlsx
+++ b/metadata/lambda_conversion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hputnam/MyProjects/Meth_Compare/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF5AF9F-D491-8840-9D07-4594D4AE551F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BA1C6A-7BE5-E24B-B870-AF06B8396B3B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="860" windowWidth="19720" windowHeight="19200" xr2:uid="{FCA444CC-6BD9-9E4F-A0C4-F7BD52B2780A}"/>
+    <workbookView xWindow="440" yWindow="860" windowWidth="15680" windowHeight="19080" xr2:uid="{FCA444CC-6BD9-9E4F-A0C4-F7BD52B2780A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="58">
   <si>
     <t>% methylation (context) = 100 * methylated Cs (context) / (methylated Cs (context) + unmethylated Cs (context)).</t>
   </si>
@@ -175,6 +175,36 @@
   </si>
   <si>
     <t>https://gannet.fish.washington.edu/seashell/bu-mox/scrubbed/032820-lambda/lambda_tg/Meth5_R1_001_val_1_bismark_bt2_PE_report.txt</t>
+  </si>
+  <si>
+    <t>https://gannet.fish.washington.edu/seashell/bu-mox/scrubbed/032820-lambda/lambda_tg/Meth6_R1_001_val_1_bismark_bt2_PE_report.txt</t>
+  </si>
+  <si>
+    <t>https://gannet.fish.washington.edu/seashell/bu-mox/scrubbed/032820-lambda/lambda_tg/Meth7_R1_001_val_1_bismark_bt2_PE_report.txt</t>
+  </si>
+  <si>
+    <t>https://gannet.fish.washington.edu/seashell/bu-mox/scrubbed/032820-lambda/lambda_tg/Meth8_R1_001_val_1_bismark_bt2_PE_report.txt</t>
+  </si>
+  <si>
+    <t>https://gannet.fish.washington.edu/seashell/bu-mox/scrubbed/032820-lambda/lambda_tg/Meth9_R1_001_val_1_bismark_bt2_PE_report.txt</t>
+  </si>
+  <si>
+    <t>Pact WGBS</t>
+  </si>
+  <si>
+    <t>Pact RRBS</t>
+  </si>
+  <si>
+    <t>Pact MBDBS</t>
+  </si>
+  <si>
+    <t>Mcap WGBS</t>
+  </si>
+  <si>
+    <t>Mcap RRBS</t>
+  </si>
+  <si>
+    <t>Mcap MBDBS</t>
   </si>
 </sst>
 </file>
@@ -256,7 +286,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -264,6 +294,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -582,13 +613,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DFAA147-CBC3-2142-8F23-446CB55231B3}">
   <dimension ref="A1:H126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="6" width="10.83203125" style="3"/>
+    <col min="7" max="7" width="12.5" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -785,6 +818,9 @@
       <c r="G10" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="H10" s="6" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -807,6 +843,9 @@
       <c r="G11" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="H11" s="6" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -829,6 +868,9 @@
       <c r="G12" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="H12" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -850,6 +892,9 @@
       </c>
       <c r="G13" s="3" t="s">
         <v>20</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1100,7 +1145,7 @@
       <c r="G25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H25" s="7">
+      <c r="H25" s="8">
         <f>E7*100</f>
         <v>98.780098341657862</v>
       </c>
@@ -1126,7 +1171,7 @@
       <c r="G26" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H26" s="8">
         <f>E14*100</f>
         <v>98.252618201775135</v>
       </c>
@@ -1152,7 +1197,7 @@
       <c r="G27" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H27" s="8">
         <f>E21*100</f>
         <v>98.774902837590702</v>
       </c>
@@ -1176,7 +1221,7 @@
       <c r="G28" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="8">
         <f>E28*100</f>
         <v>99.238640862261349</v>
       </c>
@@ -1185,7 +1230,7 @@
       <c r="G29" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="7">
+      <c r="H29" s="8">
         <f>E35*100</f>
         <v>99.060846860939421</v>
       </c>
@@ -1209,9 +1254,9 @@
       <c r="G30" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="7" t="e">
+      <c r="H30" s="8">
         <f>E42*100</f>
-        <v>#DIV/0!</v>
+        <v>99.177015880727794</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.25">
@@ -1235,9 +1280,9 @@
       <c r="G31" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H31" s="7" t="e">
+      <c r="H31" s="8">
         <f>E49*100</f>
-        <v>#DIV/0!</v>
+        <v>98.673422282272142</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.25">
@@ -1261,9 +1306,9 @@
       <c r="G32" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H32" s="7" t="e">
+      <c r="H32" s="8">
         <f>E56*100</f>
-        <v>#DIV/0!</v>
+        <v>98.516391702300297</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.25">
@@ -1287,9 +1332,9 @@
       <c r="G33" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H33" s="7" t="e">
+      <c r="H33" s="8">
         <f>E63*100</f>
-        <v>#DIV/0!</v>
+        <v>98.510190136241931</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.25">
@@ -1313,7 +1358,7 @@
       <c r="G34" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H34" s="7">
+      <c r="H34" s="8">
         <f>E70*100</f>
         <v>98.633954360140237</v>
       </c>
@@ -1337,7 +1382,7 @@
       <c r="G35" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H35" s="7">
+      <c r="H35" s="8">
         <f>E77*100</f>
         <v>98.575443656248623</v>
       </c>
@@ -1346,7 +1391,7 @@
       <c r="G36" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H36" s="7">
+      <c r="H36" s="8">
         <f>E84*100</f>
         <v>98.6977058262204</v>
       </c>
@@ -1370,95 +1415,111 @@
       <c r="G37" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H37" s="7">
+      <c r="H37" s="8">
         <f>E91*100</f>
         <v>99.256847881360372</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
+      <c r="B38" s="1">
+        <v>8969121</v>
+      </c>
+      <c r="C38" s="1">
+        <v>262346185</v>
+      </c>
       <c r="D38" s="3">
         <f>SUM(B38:C38)</f>
-        <v>0</v>
-      </c>
-      <c r="E38" s="3" t="e">
+        <v>271315306</v>
+      </c>
+      <c r="E38" s="3">
         <f>B38/D38</f>
-        <v>#DIV/0!</v>
+        <v>3.3057924863258543E-2</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H38" s="7">
+      <c r="H38" s="8">
         <f>E98*100</f>
         <v>99.242773001432965</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
+      <c r="B39" s="1">
+        <v>1269417</v>
+      </c>
+      <c r="C39" s="1">
+        <v>217295520</v>
+      </c>
       <c r="D39" s="3">
         <f t="shared" ref="D39:D41" si="10">SUM(B39:C39)</f>
-        <v>0</v>
-      </c>
-      <c r="E39" s="3" t="e">
+        <v>218564937</v>
+      </c>
+      <c r="E39" s="3">
         <f t="shared" ref="E39:E41" si="11">B39/D39</f>
-        <v>#DIV/0!</v>
+        <v>5.807962692570401E-3</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H39" s="7">
+      <c r="H39" s="8">
         <f>E105*100</f>
         <v>99.248453087484407</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
+      <c r="B40" s="1">
+        <v>3356012</v>
+      </c>
+      <c r="C40" s="1">
+        <v>344585831</v>
+      </c>
       <c r="D40" s="3">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="E40" s="3" t="e">
+        <v>347941843</v>
+      </c>
+      <c r="E40" s="3">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>9.6453245492523296E-3</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H40" s="7">
+      <c r="H40" s="8">
         <f>E112*100</f>
         <v>98.729652435519725</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
+      <c r="B41" s="1">
+        <v>38087</v>
+      </c>
+      <c r="C41" s="1">
+        <v>114427</v>
+      </c>
       <c r="D41" s="3">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="E41" s="3" t="e">
+        <v>152514</v>
+      </c>
+      <c r="E41" s="3">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>0.24972789383269733</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H41" s="7">
+      <c r="H41" s="8">
         <f>E119*100</f>
         <v>98.798967642262852</v>
       </c>
@@ -1469,20 +1530,20 @@
       </c>
       <c r="C42" s="3">
         <f>SUM(C39:C41)</f>
-        <v>0</v>
+        <v>561995778</v>
       </c>
       <c r="D42" s="3">
         <f>SUM(D39:D41)</f>
-        <v>0</v>
-      </c>
-      <c r="E42" s="3" t="e">
+        <v>566659294</v>
+      </c>
+      <c r="E42" s="3">
         <f>C42/D42</f>
-        <v>#DIV/0!</v>
+        <v>0.99177015880727792</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H42" s="7">
+      <c r="H42" s="8">
         <f>E126*100</f>
         <v>98.74865916874991</v>
       </c>
@@ -1506,96 +1567,142 @@
       <c r="G44" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H44" s="3" t="e">
-        <f ca="1">mean(H25:H42)</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H44" s="7">
+        <f>AVERAGE(H25:H42)</f>
+        <v>98.828699120288121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
+      <c r="B45" s="1">
+        <v>355102</v>
+      </c>
+      <c r="C45" s="1">
+        <v>29666526</v>
+      </c>
       <c r="D45" s="3">
         <f>SUM(B45:C45)</f>
-        <v>0</v>
-      </c>
-      <c r="E45" s="3" t="e">
+        <v>30021628</v>
+      </c>
+      <c r="E45" s="3">
         <f>B45/D45</f>
-        <v>#DIV/0!</v>
+        <v>1.1828205985364951E-2</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H45" s="3" t="e">
+      <c r="H45" s="7">
         <f>STDEV(H25:H42)/(SQRT(COUNT(H25:H42)))</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+        <v>7.164671616408691E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
+      <c r="B46" s="1">
+        <v>292359</v>
+      </c>
+      <c r="C46" s="1">
+        <v>24937022</v>
+      </c>
       <c r="D46" s="3">
         <f t="shared" ref="D46:D48" si="12">SUM(B46:C46)</f>
-        <v>0</v>
-      </c>
-      <c r="E46" s="3" t="e">
+        <v>25229381</v>
+      </c>
+      <c r="E46" s="3">
         <f t="shared" ref="E46:E48" si="13">B46/D46</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1.1588036979583447E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
+      <c r="B47" s="1">
+        <v>599722</v>
+      </c>
+      <c r="C47" s="1">
+        <v>44901914</v>
+      </c>
       <c r="D47" s="3">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="E47" s="3" t="e">
+        <v>45501636</v>
+      </c>
+      <c r="E47" s="3">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1.3180229387796078E-2</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H47" s="8">
+        <f>AVERAGE(H25:H27)</f>
+        <v>98.602539793674566</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
+      <c r="B48" s="1">
+        <v>50479</v>
+      </c>
+      <c r="C48" s="1">
+        <v>270504</v>
+      </c>
       <c r="D48" s="3">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="E48" s="3" t="e">
+        <v>320983</v>
+      </c>
+      <c r="E48" s="3">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.15726378032481472</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H48" s="8">
+        <f>AVERAGE(H28:H30)</f>
+        <v>99.15883453464285</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C49" s="3">
         <f>SUM(C46:C48)</f>
-        <v>0</v>
+        <v>70109440</v>
       </c>
       <c r="D49" s="3">
         <f>SUM(D46:D48)</f>
-        <v>0</v>
-      </c>
-      <c r="E49" s="3" t="e">
+        <v>71052000</v>
+      </c>
+      <c r="E49" s="3">
         <f>C49/D49</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.98673422282272139</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H49" s="8">
+        <f>AVERAGE(H31:H33)</f>
+        <v>98.566668040271452</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G50" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H50" s="8">
+        <f>AVERAGE(H34:H36)</f>
+        <v>98.635701280869753</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>19</v>
       </c>
@@ -1611,85 +1718,115 @@
       <c r="E51" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G51" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H51" s="8">
+        <f>AVERAGE(H37:H39)</f>
+        <v>99.249357990092577</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
+      <c r="B52" s="1">
+        <v>408609</v>
+      </c>
+      <c r="C52" s="1">
+        <v>29942775</v>
+      </c>
       <c r="D52" s="3">
         <f>SUM(B52:C52)</f>
-        <v>0</v>
-      </c>
-      <c r="E52" s="3" t="e">
+        <v>30351384</v>
+      </c>
+      <c r="E52" s="3">
         <f>B52/D52</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1.3462615082066769E-2</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H52" s="8">
+        <f>AVERAGE(H40:H42)</f>
+        <v>98.7590930821775</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
+      <c r="B53" s="1">
+        <v>332944</v>
+      </c>
+      <c r="C53" s="1">
+        <v>25190219</v>
+      </c>
       <c r="D53" s="3">
         <f t="shared" ref="D53:D55" si="14">SUM(B53:C53)</f>
-        <v>0</v>
-      </c>
-      <c r="E53" s="3" t="e">
+        <v>25523163</v>
+      </c>
+      <c r="E53" s="3">
         <f t="shared" ref="E53:E55" si="15">B53/D53</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1.3044778188346014E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
+      <c r="B54" s="1">
+        <v>674102</v>
+      </c>
+      <c r="C54" s="1">
+        <v>45438950</v>
+      </c>
       <c r="D54" s="3">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="E54" s="3" t="e">
+        <v>46113052</v>
+      </c>
+      <c r="E54" s="3">
         <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1.4618464204017552E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
+      <c r="B55" s="1">
+        <v>60803</v>
+      </c>
+      <c r="C55" s="1">
+        <v>279460</v>
+      </c>
       <c r="D55" s="3">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="E55" s="3" t="e">
+        <v>340263</v>
+      </c>
+      <c r="E55" s="3">
         <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.17869412777763083</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C56" s="3">
         <f>SUM(C53:C55)</f>
-        <v>0</v>
+        <v>70908629</v>
       </c>
       <c r="D56" s="3">
         <f>SUM(D53:D55)</f>
-        <v>0</v>
-      </c>
-      <c r="E56" s="3" t="e">
+        <v>71976478</v>
+      </c>
+      <c r="E56" s="3">
         <f>C56/D56</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.98516391702300299</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>20</v>
       </c>
@@ -1706,81 +1843,97 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
+      <c r="B59" s="1">
+        <v>371121</v>
+      </c>
+      <c r="C59" s="1">
+        <v>27272922</v>
+      </c>
       <c r="D59" s="3">
         <f>SUM(B59:C59)</f>
-        <v>0</v>
-      </c>
-      <c r="E59" s="3" t="e">
+        <v>27644043</v>
+      </c>
+      <c r="E59" s="3">
         <f>B59/D59</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1.3424989969810132E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
+      <c r="B60" s="1">
+        <v>318297</v>
+      </c>
+      <c r="C60" s="1">
+        <v>22972831</v>
+      </c>
       <c r="D60" s="3">
         <f t="shared" ref="D60:D62" si="16">SUM(B60:C60)</f>
-        <v>0</v>
-      </c>
-      <c r="E60" s="3" t="e">
+        <v>23291128</v>
+      </c>
+      <c r="E60" s="3">
         <f t="shared" ref="E60:E62" si="17">B60/D60</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1.3666019095339651E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
+      <c r="B61" s="1">
+        <v>604062</v>
+      </c>
+      <c r="C61" s="1">
+        <v>41800018</v>
+      </c>
       <c r="D61" s="3">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="E61" s="3" t="e">
+        <v>42404080</v>
+      </c>
+      <c r="E61" s="3">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1.4245374501698892E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
+      <c r="B62" s="1">
+        <v>61561</v>
+      </c>
+      <c r="C62" s="1">
+        <v>286558</v>
+      </c>
       <c r="D62" s="3">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="E62" s="3" t="e">
+        <v>348119</v>
+      </c>
+      <c r="E62" s="3">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.17683895449544551</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C63" s="3">
         <f>SUM(C60:C62)</f>
-        <v>0</v>
+        <v>65059407</v>
       </c>
       <c r="D63" s="3">
         <f>SUM(D60:D62)</f>
-        <v>0</v>
-      </c>
-      <c r="E63" s="3" t="e">
+        <v>66043327</v>
+      </c>
+      <c r="E63" s="3">
         <f>C63/D63</f>
-        <v>#DIV/0!</v>
+        <v>0.98510190136241926</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -2794,6 +2947,10 @@
     <hyperlink ref="H8" r:id="rId13" xr:uid="{87B48C2E-B7C4-A040-A188-766CE0685372}"/>
     <hyperlink ref="G4" r:id="rId14" xr:uid="{0C453366-B304-EC4D-87DA-F3DC362F189D}"/>
     <hyperlink ref="H9" r:id="rId15" xr:uid="{72ED546C-BA79-564A-BFFF-C0B61FAF9425}"/>
+    <hyperlink ref="H10" r:id="rId16" xr:uid="{43A101DD-6761-704A-8960-0A412689399D}"/>
+    <hyperlink ref="H11" r:id="rId17" xr:uid="{B99711EB-CFC4-0D43-88C1-F40D6BD7203C}"/>
+    <hyperlink ref="H12" r:id="rId18" xr:uid="{1D091A3D-F808-684E-B9C5-3C2EA0CEB0B7}"/>
+    <hyperlink ref="H13" r:id="rId19" xr:uid="{3870558E-4EF8-5145-AAB2-890F2808C264}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updating lambda and circos
</commit_message>
<xml_diff>
--- a/metadata/lambda_conversion.xlsx
+++ b/metadata/lambda_conversion.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hputnam/MyProjects/Meth_Compare/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BA1C6A-7BE5-E24B-B870-AF06B8396B3B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8E07B3-C235-D948-A155-74352BA51AD8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="860" windowWidth="15680" windowHeight="19080" xr2:uid="{FCA444CC-6BD9-9E4F-A0C4-F7BD52B2780A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -212,7 +212,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -295,7 +295,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -614,7 +614,7 @@
   <dimension ref="A1:H126"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+      <selection activeCell="H25" sqref="H25:H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1145,7 +1145,7 @@
       <c r="G25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H25" s="8">
+      <c r="H25" s="7">
         <f>E7*100</f>
         <v>98.780098341657862</v>
       </c>
@@ -1171,7 +1171,7 @@
       <c r="G26" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="8">
+      <c r="H26" s="7">
         <f>E14*100</f>
         <v>98.252618201775135</v>
       </c>
@@ -1197,7 +1197,7 @@
       <c r="G27" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="8">
+      <c r="H27" s="7">
         <f>E21*100</f>
         <v>98.774902837590702</v>
       </c>
@@ -1221,7 +1221,7 @@
       <c r="G28" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="8">
+      <c r="H28" s="7">
         <f>E28*100</f>
         <v>99.238640862261349</v>
       </c>
@@ -1230,7 +1230,7 @@
       <c r="G29" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="8">
+      <c r="H29" s="7">
         <f>E35*100</f>
         <v>99.060846860939421</v>
       </c>
@@ -1254,7 +1254,7 @@
       <c r="G30" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="8">
+      <c r="H30" s="7">
         <f>E42*100</f>
         <v>99.177015880727794</v>
       </c>
@@ -1280,7 +1280,7 @@
       <c r="G31" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H31" s="8">
+      <c r="H31" s="7">
         <f>E49*100</f>
         <v>98.673422282272142</v>
       </c>
@@ -1306,7 +1306,7 @@
       <c r="G32" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H32" s="8">
+      <c r="H32" s="7">
         <f>E56*100</f>
         <v>98.516391702300297</v>
       </c>
@@ -1332,7 +1332,7 @@
       <c r="G33" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H33" s="8">
+      <c r="H33" s="7">
         <f>E63*100</f>
         <v>98.510190136241931</v>
       </c>
@@ -1358,7 +1358,7 @@
       <c r="G34" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H34" s="8">
+      <c r="H34" s="7">
         <f>E70*100</f>
         <v>98.633954360140237</v>
       </c>
@@ -1382,7 +1382,7 @@
       <c r="G35" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H35" s="8">
+      <c r="H35" s="7">
         <f>E77*100</f>
         <v>98.575443656248623</v>
       </c>
@@ -1391,7 +1391,7 @@
       <c r="G36" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H36" s="8">
+      <c r="H36" s="7">
         <f>E84*100</f>
         <v>98.6977058262204</v>
       </c>
@@ -1415,7 +1415,7 @@
       <c r="G37" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H37" s="8">
+      <c r="H37" s="7">
         <f>E91*100</f>
         <v>99.256847881360372</v>
       </c>
@@ -1441,7 +1441,7 @@
       <c r="G38" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H38" s="8">
+      <c r="H38" s="7">
         <f>E98*100</f>
         <v>99.242773001432965</v>
       </c>
@@ -1467,7 +1467,7 @@
       <c r="G39" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H39" s="8">
+      <c r="H39" s="7">
         <f>E105*100</f>
         <v>99.248453087484407</v>
       </c>
@@ -1493,7 +1493,7 @@
       <c r="G40" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H40" s="8">
+      <c r="H40" s="7">
         <f>E112*100</f>
         <v>98.729652435519725</v>
       </c>
@@ -1519,7 +1519,7 @@
       <c r="G41" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H41" s="8">
+      <c r="H41" s="7">
         <f>E119*100</f>
         <v>98.798967642262852</v>
       </c>
@@ -1543,7 +1543,7 @@
       <c r="G42" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H42" s="8">
+      <c r="H42" s="7">
         <f>E126*100</f>
         <v>98.74865916874991</v>
       </c>
@@ -2953,5 +2953,6 @@
     <hyperlink ref="H13" r:id="rId19" xr:uid="{3870558E-4EF8-5145-AAB2-890F2808C264}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>